<commit_message>
Updating the Morning Coffee breaks
</commit_message>
<xml_diff>
--- a/resources/EMNLP2015-Program-at-glance.xlsx
+++ b/resources/EMNLP2015-Program-at-glance.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19580" yWindow="840" windowWidth="24720" windowHeight="19240" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="12900" yWindow="0" windowWidth="22380" windowHeight="19240" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="131">
   <si>
     <t>Morning
 Tutorials</t>
@@ -1303,6 +1303,9 @@
   </si>
   <si>
     <t>15:10 - 15:40</t>
+  </si>
+  <si>
+    <t>Morning Coffee</t>
   </si>
 </sst>
 </file>
@@ -1439,7 +1442,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1830,8 +1833,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="177">
+  <cellStyleXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2009,8 +2043,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
@@ -2183,78 +2239,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
@@ -2273,9 +2257,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2300,16 +2281,10 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
@@ -2323,80 +2298,176 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="177">
+  <cellStyles count="199">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2485,6 +2556,17 @@
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2573,6 +2655,17 @@
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3349,16 +3442,16 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="41"/>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="100" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="103" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="27" t="s">
@@ -3373,10 +3466,10 @@
     </row>
     <row r="4" spans="1:12" ht="29">
       <c r="A4" s="41"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="66"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="104"/>
       <c r="F4" s="57" t="s">
         <v>14</v>
       </c>
@@ -3393,10 +3486,10 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="41"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="66"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="104"/>
       <c r="F5" s="49" t="s">
         <v>62</v>
       </c>
@@ -3409,10 +3502,10 @@
     </row>
     <row r="6" spans="1:12" ht="58">
       <c r="A6" s="42"/>
-      <c r="B6" s="64"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="67"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="105"/>
       <c r="F6" s="44" t="s">
         <v>44</v>
       </c>
@@ -3457,16 +3550,16 @@
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
       <c r="A8" s="42"/>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="71" t="s">
+      <c r="C8" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="71" t="s">
+      <c r="E8" s="109" t="s">
         <v>2</v>
       </c>
       <c r="F8" s="52"/>
@@ -3481,10 +3574,10 @@
     </row>
     <row r="9" spans="1:12" ht="58">
       <c r="A9" s="42"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="72"/>
+      <c r="B9" s="101"/>
+      <c r="C9" s="110"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="110"/>
       <c r="F9" s="44" t="s">
         <v>50</v>
       </c>
@@ -3507,10 +3600,10 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="42"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="72"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="101"/>
+      <c r="E10" s="110"/>
       <c r="F10" s="49" t="s">
         <v>63</v>
       </c>
@@ -3523,10 +3616,10 @@
     </row>
     <row r="11" spans="1:12" ht="58">
       <c r="A11" s="42"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="73"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="111"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="111"/>
       <c r="F11" s="44" t="s">
         <v>56</v>
       </c>
@@ -3735,16 +3828,16 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="41"/>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="100" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="71" t="s">
+      <c r="E3" s="109" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="27" t="s">
@@ -3759,10 +3852,10 @@
     </row>
     <row r="4" spans="1:12" ht="29">
       <c r="A4" s="41"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="72"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="110"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="110"/>
       <c r="F4" s="57" t="s">
         <v>68</v>
       </c>
@@ -3779,10 +3872,10 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="41"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="72"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="110"/>
       <c r="F5" s="49" t="s">
         <v>62</v>
       </c>
@@ -3795,10 +3888,10 @@
     </row>
     <row r="6" spans="1:12" ht="58">
       <c r="A6" s="42"/>
-      <c r="B6" s="64"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="73"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="111"/>
       <c r="F6" s="44" t="s">
         <v>71</v>
       </c>
@@ -3821,54 +3914,54 @@
     </row>
     <row r="7" spans="1:12" ht="17" customHeight="1">
       <c r="A7" s="42"/>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="120" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="80" t="s">
+      <c r="C7" s="121"/>
+      <c r="D7" s="121"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="112" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="84" t="s">
+      <c r="G7" s="113"/>
+      <c r="H7" s="118" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="80" t="s">
+      <c r="I7" s="119"/>
+      <c r="J7" s="112" t="s">
         <v>77</v>
       </c>
-      <c r="K7" s="82"/>
+      <c r="K7" s="116"/>
       <c r="L7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="32" customHeight="1">
       <c r="A8" s="42"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="79"/>
+      <c r="B8" s="122"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="114"/>
+      <c r="G8" s="115"/>
       <c r="H8" s="61" t="s">
         <v>95</v>
       </c>
       <c r="I8" s="58"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="83"/>
+      <c r="J8" s="114"/>
+      <c r="K8" s="117"/>
       <c r="L8" s="35"/>
     </row>
     <row r="9" spans="1:12" ht="58">
       <c r="A9" s="42"/>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="71" t="s">
+      <c r="C9" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="68" t="s">
+      <c r="D9" s="106" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="71" t="s">
+      <c r="E9" s="109" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="44" t="s">
@@ -3893,10 +3986,10 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="42"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="72"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="107"/>
+      <c r="E10" s="110"/>
       <c r="F10" s="49" t="s">
         <v>96</v>
       </c>
@@ -3909,10 +4002,10 @@
     </row>
     <row r="11" spans="1:12" ht="58">
       <c r="A11" s="42"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="73"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="111"/>
+      <c r="D11" s="108"/>
+      <c r="E11" s="111"/>
       <c r="F11" s="44" t="s">
         <v>84</v>
       </c>
@@ -4041,18 +4134,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
     <mergeCell ref="F7:G8"/>
     <mergeCell ref="J7:K8"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="E3:E6"/>
     <mergeCell ref="C3:C6"/>
     <mergeCell ref="D3:D6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4066,14 +4159,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
@@ -4097,369 +4189,369 @@
       <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:12" ht="22" customHeight="1" thickBot="1">
-      <c r="A2" s="127"/>
-      <c r="B2" s="130" t="s">
+      <c r="A2" s="91"/>
+      <c r="B2" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="131"/>
-      <c r="D2" s="132" t="s">
+      <c r="C2" s="95"/>
+      <c r="D2" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="131"/>
-      <c r="F2" s="132" t="s">
+      <c r="E2" s="95"/>
+      <c r="F2" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="131"/>
-      <c r="H2" s="132" t="s">
+      <c r="G2" s="95"/>
+      <c r="H2" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="131"/>
-      <c r="J2" s="132" t="s">
+      <c r="I2" s="95"/>
+      <c r="J2" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="133"/>
+      <c r="K2" s="97"/>
       <c r="L2" s="35"/>
     </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" thickTop="1">
-      <c r="A3" s="127"/>
-      <c r="B3" s="113" t="s">
+    <row r="3" spans="1:12" ht="16" thickTop="1">
+      <c r="A3" s="91"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="92" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="35"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="91"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="88" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="35"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" customHeight="1" thickBot="1">
+      <c r="A5" s="91"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="92" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="93"/>
+      <c r="K5" s="93"/>
+      <c r="L5" s="35"/>
+    </row>
+    <row r="6" spans="1:12" ht="16" thickTop="1">
+      <c r="A6" s="91"/>
+      <c r="B6" s="137" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="120" t="s">
+      <c r="C6" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="113" t="s">
+      <c r="D6" s="140" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="120" t="s">
+      <c r="E6" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="128" t="s">
-        <v>124</v>
-      </c>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129"/>
-      <c r="I3" s="129"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="129"/>
-      <c r="L3" s="35"/>
-    </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1">
-      <c r="A4" s="127"/>
-      <c r="B4" s="113"/>
-      <c r="C4" s="120"/>
-      <c r="D4" s="113"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="124" t="s">
-        <v>125</v>
-      </c>
-      <c r="G4" s="125"/>
-      <c r="H4" s="125"/>
-      <c r="I4" s="125"/>
-      <c r="J4" s="125"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="35"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="127"/>
-      <c r="B5" s="113"/>
-      <c r="C5" s="120"/>
-      <c r="D5" s="113"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="134" t="s">
+      <c r="F6" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="135"/>
-      <c r="H5" s="92" t="s">
+      <c r="G6" s="99"/>
+      <c r="H6" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="I5" s="90"/>
-      <c r="J5" s="92" t="s">
+      <c r="I6" s="66"/>
+      <c r="J6" s="68" t="s">
         <v>112</v>
       </c>
-      <c r="K5" s="92"/>
-      <c r="L5" s="35"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="41"/>
-      <c r="B6" s="113"/>
-      <c r="C6" s="120"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="120"/>
-      <c r="F6" s="100" t="s">
+      <c r="K6" s="68"/>
+      <c r="L6" s="35"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="41"/>
+      <c r="B7" s="135"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="133"/>
+      <c r="E7" s="128"/>
+      <c r="F7" s="75" t="s">
         <v>123</v>
       </c>
-      <c r="G6" s="91"/>
-      <c r="H6" s="100" t="s">
+      <c r="G7" s="67"/>
+      <c r="H7" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="100" t="s">
+      <c r="I7" s="67"/>
+      <c r="J7" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="K6" s="100"/>
-      <c r="L6" s="35"/>
-    </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1">
-      <c r="A7" s="41"/>
-      <c r="B7" s="113"/>
-      <c r="C7" s="120"/>
-      <c r="D7" s="113"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="50" t="s">
+      <c r="K7" s="75"/>
+      <c r="L7" s="35"/>
+    </row>
+    <row r="8" spans="1:12" ht="15" customHeight="1">
+      <c r="A8" s="41"/>
+      <c r="B8" s="135"/>
+      <c r="C8" s="128"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="128"/>
+      <c r="F8" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="G7" s="122"/>
-      <c r="H7" s="122"/>
-      <c r="I7" s="122"/>
-      <c r="J7" s="122"/>
-      <c r="K7" s="123"/>
-      <c r="L7" s="35"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="41"/>
-      <c r="B8" s="113"/>
-      <c r="C8" s="120"/>
-      <c r="D8" s="113"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="124" t="s">
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="35"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="41"/>
+      <c r="B9" s="135"/>
+      <c r="C9" s="128"/>
+      <c r="D9" s="133"/>
+      <c r="E9" s="128"/>
+      <c r="F9" s="88" t="s">
         <v>127</v>
       </c>
-      <c r="G8" s="125"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="125"/>
-      <c r="J8" s="125"/>
-      <c r="K8" s="126"/>
-      <c r="L8" s="35"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="42"/>
-      <c r="B9" s="113"/>
-      <c r="C9" s="120"/>
-      <c r="D9" s="113"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="101" t="s">
-        <v>97</v>
-      </c>
-      <c r="G9" s="88"/>
-      <c r="H9" s="101" t="s">
-        <v>99</v>
-      </c>
-      <c r="I9" s="88"/>
-      <c r="J9" s="101" t="s">
-        <v>100</v>
-      </c>
-      <c r="K9" s="107"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="90"/>
       <c r="L9" s="35"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="42"/>
-      <c r="B10" s="114"/>
-      <c r="C10" s="121"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="121"/>
-      <c r="F10" s="102" t="s">
+      <c r="B10" s="135"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="128"/>
+      <c r="F10" s="76" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" s="64"/>
+      <c r="H10" s="76" t="s">
+        <v>99</v>
+      </c>
+      <c r="I10" s="64"/>
+      <c r="J10" s="76" t="s">
+        <v>100</v>
+      </c>
+      <c r="K10" s="80"/>
+      <c r="L10" s="35"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="42"/>
+      <c r="B11" s="135"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="133"/>
+      <c r="E11" s="128"/>
+      <c r="F11" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="G10" s="98"/>
-      <c r="H10" s="102" t="s">
+      <c r="G11" s="73"/>
+      <c r="H11" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="I10" s="98"/>
-      <c r="J10" s="102" t="s">
+      <c r="I11" s="73"/>
+      <c r="J11" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="K10" s="86"/>
-      <c r="L10" s="35"/>
-    </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1">
-      <c r="A11" s="42"/>
-      <c r="B11" s="75" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="75" t="s">
+      <c r="K11" s="62"/>
+      <c r="L11" s="35"/>
+    </row>
+    <row r="12" spans="1:12" ht="15" customHeight="1">
+      <c r="A12" s="42"/>
+      <c r="B12" s="135"/>
+      <c r="C12" s="129"/>
+      <c r="D12" s="133"/>
+      <c r="E12" s="128"/>
+      <c r="F12" s="121" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="76"/>
-      <c r="H11" s="106" t="s">
+      <c r="G12" s="113"/>
+      <c r="H12" s="132" t="s">
         <v>65</v>
       </c>
-      <c r="I11" s="85"/>
-      <c r="J11" s="75" t="s">
+      <c r="I12" s="119"/>
+      <c r="J12" s="121" t="s">
         <v>77</v>
       </c>
-      <c r="K11" s="75"/>
-      <c r="L11" s="35"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="42"/>
-      <c r="B12" s="103"/>
-      <c r="C12" s="103"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="103"/>
-      <c r="G12" s="93"/>
-      <c r="H12" s="92" t="s">
-        <v>113</v>
-      </c>
-      <c r="I12" s="90"/>
-      <c r="J12" s="103"/>
-      <c r="K12" s="103"/>
+      <c r="K12" s="121"/>
       <c r="L12" s="35"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="42"/>
-      <c r="B13" s="78"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="100" t="s">
+      <c r="B13" s="120" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="121"/>
+      <c r="D13" s="121"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="130"/>
+      <c r="G13" s="131"/>
+      <c r="H13" s="68" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" s="66"/>
+      <c r="J13" s="130"/>
+      <c r="K13" s="130"/>
+      <c r="L13" s="35"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="42"/>
+      <c r="B14" s="139"/>
+      <c r="C14" s="130"/>
+      <c r="D14" s="130"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="115"/>
+      <c r="H14" s="75" t="s">
         <v>114</v>
       </c>
-      <c r="I13" s="91"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="35"/>
-    </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1">
-      <c r="A14" s="42"/>
-      <c r="B14" s="112" t="s">
+      <c r="I14" s="67"/>
+      <c r="J14" s="123"/>
+      <c r="K14" s="123"/>
+      <c r="L14" s="35"/>
+    </row>
+    <row r="15" spans="1:12" ht="15" customHeight="1">
+      <c r="A15" s="42"/>
+      <c r="B15" s="122"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="115"/>
+      <c r="F15" s="76" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" s="64"/>
+      <c r="H15" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="I15" s="64"/>
+      <c r="J15" s="76" t="s">
+        <v>104</v>
+      </c>
+      <c r="K15" s="80"/>
+      <c r="L15" s="35"/>
+    </row>
+    <row r="16" spans="1:12" ht="29" customHeight="1">
+      <c r="A16" s="42"/>
+      <c r="B16" s="134" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="119" t="s">
+      <c r="C16" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="115" t="s">
+      <c r="D16" s="124" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="119" t="s">
+      <c r="E16" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="101" t="s">
-        <v>102</v>
-      </c>
-      <c r="G14" s="88"/>
-      <c r="H14" s="101" t="s">
-        <v>103</v>
-      </c>
-      <c r="I14" s="88"/>
-      <c r="J14" s="101" t="s">
-        <v>104</v>
-      </c>
-      <c r="K14" s="107"/>
-      <c r="L14" s="35"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="42"/>
-      <c r="B15" s="113"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="102" t="s">
+      <c r="F16" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="G15" s="98"/>
-      <c r="H15" s="102" t="s">
+      <c r="G16" s="73"/>
+      <c r="H16" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="I15" s="98"/>
-      <c r="J15" s="102" t="s">
+      <c r="I16" s="73"/>
+      <c r="J16" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="K15" s="86"/>
-      <c r="L15" s="35"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="42"/>
-      <c r="B16" s="113"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="50" t="s">
-        <v>128</v>
-      </c>
-      <c r="G16" s="122"/>
-      <c r="H16" s="122"/>
-      <c r="I16" s="122"/>
-      <c r="J16" s="122"/>
-      <c r="K16" s="123"/>
+      <c r="K16" s="62"/>
       <c r="L16" s="35"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="42"/>
-      <c r="B17" s="113"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="116"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="124" t="s">
-        <v>129</v>
-      </c>
-      <c r="G17" s="125"/>
-      <c r="H17" s="125"/>
-      <c r="I17" s="125"/>
-      <c r="J17" s="125"/>
-      <c r="K17" s="126"/>
+      <c r="B17" s="135"/>
+      <c r="C17" s="128"/>
+      <c r="D17" s="125"/>
+      <c r="E17" s="128"/>
+      <c r="F17" s="50" t="s">
+        <v>128</v>
+      </c>
+      <c r="G17" s="86"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="87"/>
       <c r="L17" s="35"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="42"/>
-      <c r="B18" s="113"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="116"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="87" t="s">
-        <v>106</v>
-      </c>
-      <c r="G18" s="88"/>
-      <c r="H18" s="101" t="s">
-        <v>107</v>
-      </c>
-      <c r="I18" s="88"/>
-      <c r="J18" s="101" t="s">
-        <v>108</v>
-      </c>
-      <c r="K18" s="107"/>
+      <c r="B18" s="135"/>
+      <c r="C18" s="128"/>
+      <c r="D18" s="125"/>
+      <c r="E18" s="128"/>
+      <c r="F18" s="88" t="s">
+        <v>129</v>
+      </c>
+      <c r="G18" s="89"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="89"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="90"/>
       <c r="L18" s="35"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="42"/>
-      <c r="B19" s="114"/>
-      <c r="C19" s="121"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="121"/>
-      <c r="F19" s="118" t="s">
+      <c r="B19" s="135"/>
+      <c r="C19" s="128"/>
+      <c r="D19" s="125"/>
+      <c r="E19" s="128"/>
+      <c r="F19" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="G19" s="64"/>
+      <c r="H19" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="I19" s="64"/>
+      <c r="J19" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="K19" s="80"/>
+      <c r="L19" s="35"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="42"/>
+      <c r="B20" s="136"/>
+      <c r="C20" s="129"/>
+      <c r="D20" s="126"/>
+      <c r="E20" s="129"/>
+      <c r="F20" s="85" t="s">
         <v>105</v>
       </c>
-      <c r="G19" s="98"/>
-      <c r="H19" s="102" t="s">
+      <c r="G20" s="73"/>
+      <c r="H20" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="I19" s="98"/>
-      <c r="J19" s="102" t="s">
+      <c r="I20" s="73"/>
+      <c r="J20" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="K19" s="86"/>
-      <c r="L19" s="35"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="105"/>
-      <c r="J20" s="104" t="s">
-        <v>121</v>
-      </c>
-      <c r="K20" s="104"/>
+      <c r="K20" s="62"/>
       <c r="L20" s="35"/>
     </row>
     <row r="21" spans="1:12">
@@ -4470,67 +4562,69 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="89"/>
-      <c r="I21" s="105"/>
-      <c r="J21" s="100" t="s">
-        <v>122</v>
-      </c>
-      <c r="K21" s="100"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="K21" s="78"/>
       <c r="L21" s="35"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
-      <c r="C22" s="105"/>
-      <c r="D22" s="96" t="s">
-        <v>115</v>
-      </c>
-      <c r="E22" s="99"/>
-      <c r="F22" s="89"/>
-      <c r="G22" s="105"/>
-      <c r="H22" s="96" t="s">
-        <v>117</v>
-      </c>
-      <c r="I22" s="99"/>
-      <c r="J22" s="96" t="s">
-        <v>119</v>
-      </c>
-      <c r="K22" s="97"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="75" t="s">
+        <v>122</v>
+      </c>
+      <c r="K22" s="75"/>
       <c r="L22" s="35"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="109" t="s">
-        <v>116</v>
-      </c>
-      <c r="E23" s="110"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="108"/>
-      <c r="H23" s="109" t="s">
-        <v>118</v>
-      </c>
-      <c r="I23" s="110"/>
-      <c r="J23" s="109" t="s">
-        <v>120</v>
-      </c>
-      <c r="K23" s="111"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="74"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="I23" s="74"/>
+      <c r="J23" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="K23" s="72"/>
       <c r="L23" s="35"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="95"/>
-      <c r="H24" s="95"/>
-      <c r="I24" s="95"/>
-      <c r="J24" s="95"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" s="83"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="82" t="s">
+        <v>118</v>
+      </c>
+      <c r="I24" s="83"/>
+      <c r="J24" s="82" t="s">
+        <v>120</v>
+      </c>
+      <c r="K24" s="84"/>
+      <c r="L24" s="35"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="5"/>
@@ -4539,10 +4633,10 @@
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="95"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
@@ -4553,7 +4647,7 @@
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="G26" s="70"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
@@ -4588,20 +4682,34 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="B11:E13"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="F11:G13"/>
-    <mergeCell ref="J11:K13"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="D3:D10"/>
-    <mergeCell ref="E3:E10"/>
+    <mergeCell ref="J12:K14"/>
+    <mergeCell ref="B13:E15"/>
+    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="C6:C12"/>
+    <mergeCell ref="D6:D12"/>
+    <mergeCell ref="E6:E12"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="D16:D20"/>
+    <mergeCell ref="E16:E20"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="F12:G14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Small change in the schedule at a glance
</commit_message>
<xml_diff>
--- a/resources/EMNLP2015-Program-at-glance.xlsx
+++ b/resources/EMNLP2015-Program-at-glance.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12900" yWindow="0" windowWidth="22380" windowHeight="19240" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="26660" yWindow="960" windowWidth="22380" windowHeight="19240" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1201,9 +1201,6 @@
     <t>Parallel Session 1</t>
   </si>
   <si>
-    <t>10:00 - 12:10</t>
-  </si>
-  <si>
     <t>Parallel Session 4</t>
   </si>
   <si>
@@ -1306,6 +1303,9 @@
   </si>
   <si>
     <t>Morning Coffee</t>
+  </si>
+  <si>
+    <t>10:30 - 12:10</t>
   </si>
 </sst>
 </file>
@@ -1865,8 +1865,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="199">
+  <cellStyleXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2379,18 +2387,30 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2403,17 +2423,44 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2424,50 +2471,11 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="199">
+  <cellStyles count="207">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2567,6 +2575,10 @@
     <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2666,6 +2678,10 @@
     <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3914,40 +3930,40 @@
     </row>
     <row r="7" spans="1:12" ht="17" customHeight="1">
       <c r="A7" s="42"/>
-      <c r="B7" s="120" t="s">
+      <c r="B7" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="121"/>
-      <c r="D7" s="121"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="112" t="s">
+      <c r="C7" s="113"/>
+      <c r="D7" s="113"/>
+      <c r="E7" s="114"/>
+      <c r="F7" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="113"/>
-      <c r="H7" s="118" t="s">
+      <c r="G7" s="114"/>
+      <c r="H7" s="122" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="112" t="s">
+      <c r="I7" s="123"/>
+      <c r="J7" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="K7" s="116"/>
+      <c r="K7" s="120"/>
       <c r="L7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="32" customHeight="1">
       <c r="A8" s="42"/>
-      <c r="B8" s="122"/>
-      <c r="C8" s="123"/>
-      <c r="D8" s="123"/>
-      <c r="E8" s="115"/>
-      <c r="F8" s="114"/>
-      <c r="G8" s="115"/>
+      <c r="B8" s="115"/>
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="119"/>
+      <c r="G8" s="117"/>
       <c r="H8" s="61" t="s">
         <v>95</v>
       </c>
       <c r="I8" s="58"/>
-      <c r="J8" s="114"/>
-      <c r="K8" s="117"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="121"/>
       <c r="L8" s="35"/>
     </row>
     <row r="9" spans="1:12" ht="58">
@@ -4134,18 +4150,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F7:G8"/>
+    <mergeCell ref="J7:K8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D3:D6"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:E8"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F7:G8"/>
-    <mergeCell ref="J7:K8"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D3:D6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4161,7 +4177,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -4219,7 +4237,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="92" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" s="93"/>
       <c r="H3" s="93"/>
@@ -4235,7 +4253,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="88" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G4" s="89"/>
       <c r="H4" s="89"/>
@@ -4251,7 +4269,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="92" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G5" s="93"/>
       <c r="H5" s="93"/>
@@ -4262,60 +4280,60 @@
     </row>
     <row r="6" spans="1:12" ht="16" thickTop="1">
       <c r="A6" s="91"/>
-      <c r="B6" s="137" t="s">
+      <c r="B6" s="127" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="138" t="s">
+      <c r="C6" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="140" t="s">
+      <c r="D6" s="132" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="138" t="s">
+      <c r="E6" s="129" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="98" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G6" s="99"/>
       <c r="H6" s="68" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I6" s="66"/>
       <c r="J6" s="68" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K6" s="68"/>
       <c r="L6" s="35"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="41"/>
-      <c r="B7" s="135"/>
-      <c r="C7" s="128"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="130"/>
       <c r="D7" s="133"/>
-      <c r="E7" s="128"/>
+      <c r="E7" s="130"/>
       <c r="F7" s="75" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G7" s="67"/>
       <c r="H7" s="75" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I7" s="67"/>
       <c r="J7" s="75" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K7" s="75"/>
       <c r="L7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1">
       <c r="A8" s="41"/>
-      <c r="B8" s="135"/>
-      <c r="C8" s="128"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="130"/>
       <c r="D8" s="133"/>
-      <c r="E8" s="128"/>
+      <c r="E8" s="130"/>
       <c r="F8" s="50" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G8" s="86"/>
       <c r="H8" s="86"/>
@@ -4326,12 +4344,12 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="41"/>
-      <c r="B9" s="135"/>
-      <c r="C9" s="128"/>
+      <c r="B9" s="128"/>
+      <c r="C9" s="130"/>
       <c r="D9" s="133"/>
-      <c r="E9" s="128"/>
+      <c r="E9" s="130"/>
       <c r="F9" s="88" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G9" s="89"/>
       <c r="H9" s="89"/>
@@ -4342,114 +4360,114 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="42"/>
-      <c r="B10" s="135"/>
-      <c r="C10" s="128"/>
+      <c r="B10" s="128"/>
+      <c r="C10" s="130"/>
       <c r="D10" s="133"/>
-      <c r="E10" s="128"/>
+      <c r="E10" s="130"/>
       <c r="F10" s="76" t="s">
         <v>97</v>
       </c>
       <c r="G10" s="64"/>
       <c r="H10" s="76" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I10" s="64"/>
       <c r="J10" s="76" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K10" s="80"/>
       <c r="L10" s="35"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="42"/>
-      <c r="B11" s="135"/>
-      <c r="C11" s="128"/>
+      <c r="B11" s="128"/>
+      <c r="C11" s="130"/>
       <c r="D11" s="133"/>
-      <c r="E11" s="128"/>
+      <c r="E11" s="130"/>
       <c r="F11" s="77" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="G11" s="73"/>
       <c r="H11" s="77" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="I11" s="73"/>
       <c r="J11" s="77" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K11" s="62"/>
       <c r="L11" s="35"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1">
       <c r="A12" s="42"/>
-      <c r="B12" s="135"/>
-      <c r="C12" s="129"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="131"/>
       <c r="D12" s="133"/>
-      <c r="E12" s="128"/>
-      <c r="F12" s="121" t="s">
+      <c r="E12" s="130"/>
+      <c r="F12" s="113" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="113"/>
-      <c r="H12" s="132" t="s">
+      <c r="G12" s="114"/>
+      <c r="H12" s="140" t="s">
         <v>65</v>
       </c>
-      <c r="I12" s="119"/>
-      <c r="J12" s="121" t="s">
+      <c r="I12" s="123"/>
+      <c r="J12" s="113" t="s">
         <v>77</v>
       </c>
-      <c r="K12" s="121"/>
+      <c r="K12" s="113"/>
       <c r="L12" s="35"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="42"/>
-      <c r="B13" s="120" t="s">
+      <c r="B13" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="121"/>
-      <c r="D13" s="121"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="130"/>
-      <c r="G13" s="131"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="126"/>
       <c r="H13" s="68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I13" s="66"/>
-      <c r="J13" s="130"/>
-      <c r="K13" s="130"/>
+      <c r="J13" s="124"/>
+      <c r="K13" s="124"/>
       <c r="L13" s="35"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="42"/>
-      <c r="B14" s="139"/>
-      <c r="C14" s="130"/>
-      <c r="D14" s="130"/>
-      <c r="E14" s="131"/>
-      <c r="F14" s="123"/>
-      <c r="G14" s="115"/>
+      <c r="B14" s="125"/>
+      <c r="C14" s="124"/>
+      <c r="D14" s="124"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="116"/>
+      <c r="G14" s="117"/>
       <c r="H14" s="75" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I14" s="67"/>
-      <c r="J14" s="123"/>
-      <c r="K14" s="123"/>
+      <c r="J14" s="116"/>
+      <c r="K14" s="116"/>
       <c r="L14" s="35"/>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
       <c r="A15" s="42"/>
-      <c r="B15" s="122"/>
-      <c r="C15" s="123"/>
-      <c r="D15" s="123"/>
-      <c r="E15" s="115"/>
+      <c r="B15" s="115"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="117"/>
       <c r="F15" s="76" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G15" s="64"/>
       <c r="H15" s="76" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I15" s="64"/>
       <c r="J15" s="76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K15" s="80"/>
       <c r="L15" s="35"/>
@@ -4459,37 +4477,37 @@
       <c r="B16" s="134" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="127" t="s">
+      <c r="C16" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="124" t="s">
+      <c r="D16" s="137" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="127" t="s">
+      <c r="E16" s="136" t="s">
         <v>2</v>
       </c>
       <c r="F16" s="77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G16" s="73"/>
       <c r="H16" s="77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I16" s="73"/>
       <c r="J16" s="77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K16" s="62"/>
       <c r="L16" s="35"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="42"/>
-      <c r="B17" s="135"/>
-      <c r="C17" s="128"/>
-      <c r="D17" s="125"/>
-      <c r="E17" s="128"/>
+      <c r="B17" s="128"/>
+      <c r="C17" s="130"/>
+      <c r="D17" s="138"/>
+      <c r="E17" s="130"/>
       <c r="F17" s="50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G17" s="86"/>
       <c r="H17" s="86"/>
@@ -4500,12 +4518,12 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="42"/>
-      <c r="B18" s="135"/>
-      <c r="C18" s="128"/>
-      <c r="D18" s="125"/>
-      <c r="E18" s="128"/>
+      <c r="B18" s="128"/>
+      <c r="C18" s="130"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="130"/>
       <c r="F18" s="88" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G18" s="89"/>
       <c r="H18" s="89"/>
@@ -4516,40 +4534,40 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="42"/>
-      <c r="B19" s="135"/>
-      <c r="C19" s="128"/>
-      <c r="D19" s="125"/>
-      <c r="E19" s="128"/>
+      <c r="B19" s="128"/>
+      <c r="C19" s="130"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="130"/>
       <c r="F19" s="63" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G19" s="64"/>
       <c r="H19" s="76" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I19" s="64"/>
       <c r="J19" s="76" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K19" s="80"/>
       <c r="L19" s="35"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="42"/>
-      <c r="B20" s="136"/>
-      <c r="C20" s="129"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="129"/>
+      <c r="B20" s="135"/>
+      <c r="C20" s="131"/>
+      <c r="D20" s="139"/>
+      <c r="E20" s="131"/>
       <c r="F20" s="85" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G20" s="73"/>
       <c r="H20" s="77" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I20" s="73"/>
       <c r="J20" s="77" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K20" s="62"/>
       <c r="L20" s="35"/>
@@ -4565,7 +4583,7 @@
       <c r="H21" s="65"/>
       <c r="I21" s="79"/>
       <c r="J21" s="78" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K21" s="78"/>
       <c r="L21" s="35"/>
@@ -4581,7 +4599,7 @@
       <c r="H22" s="65"/>
       <c r="I22" s="79"/>
       <c r="J22" s="75" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K22" s="75"/>
       <c r="L22" s="35"/>
@@ -4591,17 +4609,17 @@
       <c r="B23" s="5"/>
       <c r="C23" s="79"/>
       <c r="D23" s="71" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E23" s="74"/>
       <c r="F23" s="65"/>
       <c r="G23" s="79"/>
       <c r="H23" s="71" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I23" s="74"/>
       <c r="J23" s="71" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K23" s="72"/>
       <c r="L23" s="35"/>
@@ -4611,17 +4629,17 @@
       <c r="B24" s="5"/>
       <c r="C24" s="79"/>
       <c r="D24" s="82" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E24" s="83"/>
       <c r="F24" s="69"/>
       <c r="G24" s="81"/>
       <c r="H24" s="82" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I24" s="83"/>
       <c r="J24" s="82" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K24" s="84"/>
       <c r="L24" s="35"/>
@@ -4698,18 +4716,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="D16:D20"/>
+    <mergeCell ref="E16:E20"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="F12:G14"/>
     <mergeCell ref="J12:K14"/>
     <mergeCell ref="B13:E15"/>
     <mergeCell ref="B6:B12"/>
     <mergeCell ref="C6:C12"/>
     <mergeCell ref="D6:D12"/>
     <mergeCell ref="E6:E12"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="D16:D20"/>
-    <mergeCell ref="E16:E20"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="F12:G14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>